<commit_message>
Day_3 assingment 3rd commit
</commit_message>
<xml_diff>
--- a/assignments/29Nov/output/Q5_AcmeTestData.xlsx
+++ b/assignments/29Nov/output/Q5_AcmeTestData.xlsx
@@ -7,6 +7,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -1592,4 +1593,296 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
+      <x:c r="A3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5">
+      <x:c r="A8" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="A9" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5">
+      <x:c r="A10" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5">
+      <x:c r="A11" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5">
+      <x:c r="A12" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:5">
+      <x:c r="A13" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:5">
+      <x:c r="A14" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5">
+      <x:c r="A15" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="A16" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>